<commit_message>
algumas alterações para tratamento de dados posterior
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,20 +424,15 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Data de coleta:</t>
+          <t>REVENDEDORA</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>N.F</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
-        <is>
-          <t>REVENDEDORA</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
         <is>
           <t>DESTINO</t>
         </is>
@@ -446,20 +441,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>ADRIELMA DIAS nan</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>225642</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>77890000</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ADRIELMA DIAS  </t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
         <is>
           <t>Ananás - TO</t>
         </is>
@@ -468,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>RODRIGUES nan</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -478,27 +468,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">RODRIGUES  </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>ALAIDE CORDEIRO DE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>225685</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>77860000</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
-        <is>
-          <t>ALAIDE CORDEIRO DE</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>Wanderlândia - TO</t>
         </is>
@@ -507,7 +492,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>SOUSA nan</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -517,27 +502,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">SOUSA  </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>ANA CELIA MACIEL DE nan</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>225754</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>77910000</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ANA CELIA MACIEL DE  </t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
         <is>
           <t>Darcinópolis - TO</t>
         </is>
@@ -546,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>SOUSA NEGREIRO nan</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -556,27 +536,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">SOUSA NEGREIRO  </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>ANA LUCIA MARIA DA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>225758</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>77910000</t>
-        </is>
-      </c>
       <c r="C8" t="inlineStr">
-        <is>
-          <t>ANA LUCIA MARIA DA</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>Darcinópolis - TO</t>
         </is>
@@ -585,7 +560,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>SILVA nan</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -595,27 +570,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">SILVA  </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>ANDREIA DE FREITAS nan</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>225616</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>77958000</t>
-        </is>
-      </c>
       <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ANDREIA DE FREITAS  </t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
         <is>
           <t>São Bento do Tocantins - TO</t>
         </is>
@@ -624,7 +594,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>DA SILVA nan</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -634,14 +604,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">DA SILVA  </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>nan nan</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -651,27 +621,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">   </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>ANTONIA DARCIA nan</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>225674</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>77880000</t>
-        </is>
-      </c>
       <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ANTONIA DARCIA  </t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
         <is>
           <t>Xambioá - TO</t>
         </is>
@@ -680,7 +645,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>MESQUITA MARCOS nan</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -690,27 +655,22 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">MESQUITA MARCOS  </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>ANTONIO CELINALDO nan</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>225680</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>77893000</t>
-        </is>
-      </c>
       <c r="C15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ANTONIO CELINALDO  </t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
         <is>
           <t>Riachinho - TO</t>
         </is>
@@ -719,7 +679,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>PEREIRA nan</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -729,14 +689,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">PEREIRA  </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>nan nan</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -746,27 +706,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">   </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>AURORA FERNANDES E389775231 nan</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>225638</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>77890000</t>
-        </is>
-      </c>
       <c r="C18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AURORA FERNANDES E389775231  </t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
         <is>
           <t>Ananás - TO</t>
         </is>
@@ -775,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>SILVA nan</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -785,27 +740,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">SILVA  </t>
+          <t>nan</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>BEATRIZ PEREIRA nan</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>225622</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>77913000</t>
-        </is>
-      </c>
       <c r="C20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BEATRIZ PEREIRA  </t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
         <is>
           <t>Palmeiras do Tocantins - TO</t>
         </is>

</xml_diff>

<commit_message>
mudei para o pysimplegui
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,29 +424,29 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>REVENDEDORA</t>
+          <t>REVENDEDORAS</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>N.F</t>
+          <t>N.Fs</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>DESTINO</t>
+          <t xml:space="preserve">DESTINO </t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADRIELMA DIAS nan</t>
+          <t>BETILDE FERNANDES RABELO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>225642</t>
+          <t xml:space="preserve">225597 </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -458,201 +458,197 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RODRIGUES nan</t>
+          <t>CASSIANADASILVA CONCEICAO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">225667 </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Wanderlândia - TO</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ALAIDE CORDEIRO DE</t>
+          <t>CEYJANEMACIEL DA SILVA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>225685</t>
+          <t xml:space="preserve">225617 </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Wanderlândia - TO</t>
+          <t>São Bento do Tocantins - TO</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SOUSA nan</t>
+          <t>CLAUDILENELEMOS ALENCAR</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">225664 </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Darcinópolis - TO</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ANA CELIA MACIEL DE nan</t>
+          <t>CLAUDINEIA SILVA ARAUJO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>225754</t>
+          <t xml:space="preserve">225782 </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Darcinópolis - TO</t>
+          <t>Palmeiras do Tocantins - TO</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SOUSA NEGREIRO nan</t>
+          <t>CLEANE FONSECA SILVA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">225669 </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Palmeiras do Tocantins - TO</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ANA LUCIA MARIA DA</t>
+          <t>CLEOMAREUZÉBIO DOS SANTOS</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>225758</t>
+          <t xml:space="preserve">225678 </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Darcinópolis - TO</t>
+          <t>Araguanã - TO</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SILVA nan</t>
+          <t>CREUZA PEREIRA BRANDAO</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">225631 </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Nazaré - TO</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ANDREIA DE FREITAS nan</t>
+          <t>DARKLEY RIBEIRO DE BRITO DIAS</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>225616</t>
+          <t xml:space="preserve">225767 </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>São Bento do Tocantins - TO</t>
+          <t>Darcinópolis - TO</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DA SILVA nan</t>
+          <t>DAVILENE OLIVEIRA DA SILVA CHAVES</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">225633 </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Piraquê - TO</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>nan nan</t>
+          <t>DAYANY GONCALVES LIMA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">225729 </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Wanderlândia - TO</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ANTONIA DARCIA nan</t>
+          <t>DINA MARIA PORTILHO</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>225674</t>
+          <t xml:space="preserve">225688 </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Xambioá - TO</t>
+          <t>Angico - TO</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MESQUITA MARCOS nan</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>DAMASCENO</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
           <t>nan</t>
@@ -662,102 +658,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ANTONIO CELINALDO nan</t>
+          <t>DOMINGAS DA CRUZ SILVA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>225680</t>
+          <t xml:space="preserve">225656 </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Riachinho - TO</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>PEREIRA nan</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>nan nan</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>AURORA FERNANDES E389775231 nan</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>225638</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Ananás - TO</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>SILVA nan</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>BEATRIZ PEREIRA nan</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>225622</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Palmeiras do Tocantins - TO</t>
+          <t>Luzinópolis - TO</t>
         </is>
       </c>
     </row>

</xml_diff>